<commit_message>
Computions using one quadrilateral element (work in progress)
</commit_message>
<xml_diff>
--- a/displacements.xlsx
+++ b/displacements.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="295" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="305" uniqueCount="9">
   <si>
     <t>Nod</t>
   </si>
@@ -28,6 +28,18 @@
   </si>
   <si>
     <t>UY</t>
+  </si>
+  <si>
+    <t>X (Triang)</t>
+  </si>
+  <si>
+    <t>Y (Triang)</t>
+  </si>
+  <si>
+    <t>UX (Triang)</t>
+  </si>
+  <si>
+    <t>UY (Triang)</t>
   </si>
 </sst>
 </file>
@@ -80,8 +92,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="true"/>
-    <col min="2" max="2" width="4.140625" customWidth="true"/>
-    <col min="3" max="3" width="4.140625" customWidth="true"/>
+    <col min="2" max="2" width="9.5703125" customWidth="true"/>
+    <col min="3" max="3" width="9.42578125" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="14.42578125" customWidth="true"/>
   </cols>
@@ -91,16 +103,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">

</xml_diff>